<commit_message>
Convert data to csv file
</commit_message>
<xml_diff>
--- a/data/table1.xlsx
+++ b/data/table1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyu13\Documents\Projects\FIT3179\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyu13\Documents\Projects\FIT3179Wk10\FIT3179Wk10\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35130C85-DDB9-4757-B9DF-042FDCAB0818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B81B58F-E4C2-4F50-8410-ED1BE446B6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26730" yWindow="1575" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>

</xml_diff>